<commit_message>
Update monthly economic variables
1. Retail trade turnover
2. Export price index
3. Import price index
4. Employment
5. Gross wages and salaries: manufacturing and mining
6. Gross wages and salaries: main construction industry
</commit_message>
<xml_diff>
--- a/hard_data/data_monthly/variables_definitions.xlsx
+++ b/hard_data/data_monthly/variables_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Userhome\mokuneva\nowcasting_with_text\hard_data\data_monthly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3597A2C-270B-41BF-BF1D-F00C2145F88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358B6B6E-6B82-463A-8C5C-81DB5A85659C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Mnemonic</t>
   </si>
@@ -115,6 +115,42 @@
   </si>
   <si>
     <t>Hours worked: construction</t>
+  </si>
+  <si>
+    <t>RetTurn</t>
+  </si>
+  <si>
+    <t>Retail turnover excluding cars</t>
+  </si>
+  <si>
+    <t>EPI</t>
+  </si>
+  <si>
+    <t>IPI</t>
+  </si>
+  <si>
+    <t>Export price index</t>
+  </si>
+  <si>
+    <t>Import price index</t>
+  </si>
+  <si>
+    <t>Empl</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>GWMan</t>
+  </si>
+  <si>
+    <t>Gross wages and salaries: manufacturing and mining</t>
+  </si>
+  <si>
+    <t>GWConstr</t>
+  </si>
+  <si>
+    <t>Gross wages and salaries: construction</t>
   </si>
 </sst>
 </file>
@@ -432,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,21 +555,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -541,10 +577,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -552,10 +588,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -563,23 +599,89 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>